<commit_message>
update 209 patch 2
</commit_message>
<xml_diff>
--- a/data/Dialog/Drama/_tutorial.xlsx
+++ b/data/Dialog/Drama/_tutorial.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="739">
   <si>
     <t xml:space="preserve">version</t>
   </si>
@@ -4192,7 +4192,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A361" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="K359" sqref="K359"/>
+      <selection activeCell="K395" sqref="K395"/>
       <selection pane="bottomLeft" activeCell="H374" sqref="H374"/>
     </sheetView>
   </sheetViews>

</xml_diff>